<commit_message>
More fixes and so on
</commit_message>
<xml_diff>
--- a/models/data/tox_test.xlsx
+++ b/models/data/tox_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Mobius2\models\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7F18F2-40DD-4894-8E6E-7164A1B1DA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10479240-C76E-4BE2-8D1A-5034C548CF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="12735" xr2:uid="{D0E19786-DA9A-4277-8346-8F1041FBB6FD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D0E19786-DA9A-4277-8346-8F1041FBB6FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Deposition" sheetId="1" r:id="rId1"/>
@@ -396,7 +396,7 @@
   <dimension ref="A1:C10958"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,15 +420,15 @@
         <v>25569</v>
       </c>
       <c r="B3" s="2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>29221</v>
+        <v>31048</v>
       </c>
       <c r="B4" s="2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -436,7 +436,7 @@
         <v>32874</v>
       </c>
       <c r="B5" s="2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -444,7 +444,7 @@
         <v>34700</v>
       </c>
       <c r="B6" s="2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -452,7 +452,7 @@
         <v>36526</v>
       </c>
       <c r="B7" s="2">
-        <v>0.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Some refactoring of index set dependency code.
</commit_message>
<xml_diff>
--- a/models/data/tox_test.xlsx
+++ b/models/data/tox_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Mobius2\models\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10479240-C76E-4BE2-8D1A-5034C548CF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC5F909-5B87-44ED-B718-09F147FF9D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D0E19786-DA9A-4277-8346-8F1041FBB6FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D0E19786-DA9A-4277-8346-8F1041FBB6FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Deposition" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>linear_interpolate</t>
+    <t>Contaminant deposition</t>
   </si>
   <si>
-    <t>Contaminant deposition</t>
+    <t>step_interpolate</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <dimension ref="A1:C10958"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,13 +406,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -428,7 +428,7 @@
         <v>31048</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -436,7 +436,7 @@
         <v>32874</v>
       </c>
       <c r="B5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>